<commit_message>
Not sure what changed.
</commit_message>
<xml_diff>
--- a/res/rasgosdistintivos.xlsx
+++ b/res/rasgosdistintivos.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="57">
   <si>
     <t xml:space="preserve">i</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t xml:space="preserve">POSTERIOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">±</t>
   </si>
   <si>
     <t xml:space="preserve">ROUNDED</t>
@@ -271,13 +268,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -304,10 +305,10 @@
   <dimension ref="A1:AN6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -372,7 +373,7 @@
       <c r="AN1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -407,7 +408,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -442,7 +443,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -477,7 +478,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -504,16 +505,16 @@
       <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>16</v>
+      <c r="J5" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>17</v>
+      <c r="A6" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
@@ -549,7 +550,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -568,11 +569,11 @@
       <selection pane="topLeft" activeCell="AQ17" activeCellId="0" sqref="AQ17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="16.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="1" width="3.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="12" style="0" width="3.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="12" style="2" width="3.24"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -607,95 +608,95 @@
         <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -728,96 +729,96 @@
       <c r="K2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN2" s="2" t="s">
+      <c r="L2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN2" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -850,96 +851,96 @@
       <c r="K3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AH3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AK3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AM3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN3" s="2" t="s">
+      <c r="L3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1061,7 +1062,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1088,103 +1089,103 @@
       <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="W5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="X5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AG5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AH5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AI5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AK5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AL5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AM5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN5" s="2" t="s">
+      <c r="L5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN5" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>17</v>
+      <c r="A6" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
@@ -1305,8 +1306,8 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>47</v>
+      <c r="A7" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
@@ -1427,8 +1428,8 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>48</v>
+      <c r="A8" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
@@ -1549,8 +1550,8 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>49</v>
+      <c r="A9" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>12</v>
@@ -1671,8 +1672,8 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>50</v>
+      <c r="A10" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>11</v>
@@ -1776,25 +1777,25 @@
       <c r="AI10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AJ10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AK10" s="2" t="s">
+      <c r="AJ10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="AL10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AM10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN10" s="2" t="s">
+      <c r="AM10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN10" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>51</v>
+      <c r="A11" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>12</v>
@@ -1915,8 +1916,8 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>52</v>
+      <c r="A12" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>12</v>
@@ -2029,16 +2030,16 @@
       <c r="AL12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AM12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN12" s="2" t="s">
+      <c r="AM12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN12" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>53</v>
+      <c r="A13" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
@@ -2159,8 +2160,8 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>54</v>
+      <c r="A14" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>12</v>
@@ -2281,8 +2282,8 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>55</v>
+      <c r="A15" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>12</v>
@@ -2403,8 +2404,8 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>56</v>
+      <c r="A16" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>11</v>
@@ -2436,220 +2437,220 @@
       <c r="K16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="S16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="T16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="U16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="V16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="W16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="X16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Z16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AH16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AK16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AM16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN16" s="2" t="s">
+      <c r="L16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="T16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="W16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="X16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AH16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN16" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="R17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="S17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="T17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="U17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="V17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="W17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="X17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Z17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AG17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AH17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AI17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AK17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AL17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AM17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN17" s="2" t="s">
+      <c r="A17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="T17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="U17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="V17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="W17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="X17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN17" s="3" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2668,103 +2669,103 @@
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="2" style="1" width="4.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="2" style="1" width="4.98"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>47</v>
+      <c r="A2" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
@@ -2855,8 +2856,8 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>48</v>
+      <c r="A3" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
@@ -2947,8 +2948,8 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>49</v>
+      <c r="A4" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>12</v>
@@ -3039,8 +3040,8 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>50</v>
+      <c r="A5" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>12</v>
@@ -3114,25 +3115,25 @@
       <c r="Y5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Z5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA5" s="2" t="s">
+      <c r="Z5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="AB5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AC5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD5" s="2" t="s">
+      <c r="AC5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>51</v>
+      <c r="A6" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
@@ -3223,8 +3224,8 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>52</v>
+      <c r="A7" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
@@ -3307,16 +3308,16 @@
       <c r="AB7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AC7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD7" s="2" t="s">
+      <c r="AC7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD7" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>53</v>
+      <c r="A8" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>11</v>
@@ -3407,8 +3408,8 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>54</v>
+      <c r="A9" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>12</v>
@@ -3499,8 +3500,8 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>55</v>
+      <c r="A10" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>12</v>
@@ -3592,8 +3593,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>